<commit_message>
Major Bugfix - P copy issue is now removed
</commit_message>
<xml_diff>
--- a/output/2020_1023_1.xlsx
+++ b/output/2020_1023_1.xlsx
@@ -1756,11 +1756,7 @@
           <t>Kimdongwook</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>P821141793255</t>
-        </is>
-      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
           <t>Kimdongwook</t>
@@ -1903,11 +1899,7 @@
           <t>ijeou</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>P821141793255</t>
-        </is>
-      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
           <t>이정우</t>
@@ -2344,11 +2336,7 @@
           <t>philmin</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>P802143949960</t>
-        </is>
-      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
           <t>philmin</t>
@@ -3667,11 +3655,7 @@
           <t>hannahyeong</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>P851155549882</t>
-        </is>
-      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
           <t>한나형</t>

</xml_diff>